<commit_message>
Added support for longer quotes, fixed surplus numnber
</commit_message>
<xml_diff>
--- a/src/utils/spreadsheets/1.xlsx
+++ b/src/utils/spreadsheets/1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleupton/Desktop/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleupton/Documents/GitHub/witte-quote-generator-desktop/src/utils/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D19542E-7634-1144-8D8A-1CCE4DB535EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E90C383-4768-4E49-BDDF-5FBB3B2CB3A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1166,8 +1168,8 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1451,7 +1453,7 @@
         <v>37</v>
       </c>
       <c r="K16" s="70">
-        <v>1.0565</v>
+        <v>1</v>
       </c>
       <c r="L16" s="71" t="e">
         <f t="shared" ref="L16" si="2">J16*K16*0.62*1.1*costexchange</f>

</xml_diff>